<commit_message>
Diag loopback mode added (F11)
</commit_message>
<xml_diff>
--- a/PCB/v0.1 archive/C64toUSBKeyboard BOM.xlsx
+++ b/PCB/v0.1 archive/C64toUSBKeyboard BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyData\Geek Stuff\Projects\Commodore 64\Hardware\Keyboard\C64-USBKeyboard(Mine)\PCB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyData\Geek Stuff\Projects\Commodore 64\Hardware\Keyboard\C64-USBKeyboard\C64-USBKeyboard\PCB\v0.1 archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F181B40-462A-4C57-B75C-894A9B40125C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EAFDD0C-9DA7-42BD-895C-573B5747009C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="228" yWindow="2808" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="21048" windowHeight="11208" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="60">
   <si>
     <t>Qty</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>AMP connector</t>
+  </si>
+  <si>
+    <t>Sq hole/short lead/flat side/-/Cathode</t>
   </si>
 </sst>
 </file>
@@ -233,15 +236,21 @@
       <name val="Courier New,courier"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -249,16 +258,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -557,9 +584,10 @@
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -591,7 +619,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -611,7 +639,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -631,7 +659,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -648,7 +676,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -668,7 +696,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -688,7 +716,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -708,7 +736,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -739,8 +767,11 @@
       <c r="J8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -760,7 +791,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -777,7 +808,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -794,7 +825,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:11">
       <c r="A12" s="2">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Added Teensy connection headers to BOM, notes clarification
</commit_message>
<xml_diff>
--- a/PCB/v0.1 archive/C64toUSBKeyboard BOM.xlsx
+++ b/PCB/v0.1 archive/C64toUSBKeyboard BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyData\Geek Stuff\Projects\Commodore 64\Hardware\Keyboard\C64-USBKeyboard\C64-USBKeyboard\PCB\v0.1 archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A786DD-DD60-43DF-B882-1A16C0B87FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C26741-461F-494A-A5DF-EF75B2B83174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="-15645" windowWidth="19770" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="89">
   <si>
     <t>Qty</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>R2</t>
-  </si>
-  <si>
-    <t>20p Header</t>
   </si>
   <si>
     <t>J2</t>
@@ -202,9 +199,6 @@
     <t>Unused, Do Not Stuff</t>
   </si>
   <si>
-    <t>20 Position Receptacle Connector 0.100" (2.54mm) Through Hole Tin</t>
-  </si>
-  <si>
     <t>Samtec Inc.</t>
   </si>
   <si>
@@ -215,11 +209,96 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Teensy 4.1 Devel Board</t>
+  </si>
+  <si>
+    <t>RES 10K OHM 5% 1/4W AXIAL</t>
+  </si>
+  <si>
+    <t>RES 1K OHM 5% 1/4W AXIAL</t>
+  </si>
+  <si>
+    <t>Stackpole</t>
+  </si>
+  <si>
+    <t>CF14JT10K0</t>
+  </si>
+  <si>
+    <t>CF14JT10K0CT-ND</t>
+  </si>
+  <si>
+    <t>CF14JT1K00</t>
+  </si>
+  <si>
+    <t>CF14JT1K00CT-ND</t>
+  </si>
+  <si>
+    <t>3845-2N3904-ND</t>
+  </si>
+  <si>
+    <t>Fairchild</t>
+  </si>
+  <si>
+    <t>No longer manufactured, but widely available.</t>
+  </si>
+  <si>
+    <t>Multiple subs available</t>
+  </si>
+  <si>
+    <t>Allows for passthrough to use simultaneous with commodore kbd, otherwise can just use standard female or cut leads</t>
+  </si>
+  <si>
+    <t>C64toUSBKeyboard.0.1.gerbers.zip
+or   https://oshpark.com/shared_projects/wqtal8dL</t>
+  </si>
+  <si>
+    <t>v0.1</t>
+  </si>
+  <si>
+    <t>Leave this shorted, as designed</t>
+  </si>
+  <si>
+    <t>5 pin header to pass USB host signals from Teensy to PCB</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 1x24 POS 2.54mm (0.1")</t>
+  </si>
+  <si>
+    <t>Würth</t>
+  </si>
+  <si>
+    <t>61302411121</t>
+  </si>
+  <si>
+    <t>732-5331-ND</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 1x5 POS 2.54mm (0.1")</t>
+  </si>
+  <si>
+    <t>61300511121</t>
+  </si>
+  <si>
+    <t>732-5318-ND</t>
+  </si>
+  <si>
+    <t>U1- Hdr 1/2</t>
+  </si>
+  <si>
+    <t>U1- Hdr 3</t>
+  </si>
+  <si>
+    <t>24p headers</t>
+  </si>
+  <si>
+    <t>5p header</t>
   </si>
   <si>
     <r>
       <t>Teensy 3.6 would also work, but discontinued
-Teensy 4.1 with or without Ethernet will work
+Teensy 4.1 with or without Ethernet will also work
 can order</t>
     </r>
     <r>
@@ -241,61 +320,47 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> version to include soldered headers, or supply your own</t>
+      <t xml:space="preserve"> version to include soldered headers</t>
     </r>
   </si>
   <si>
-    <t>Teensy 4.1 Devel Board</t>
-  </si>
-  <si>
-    <t>RES 10K OHM 5% 1/4W AXIAL</t>
-  </si>
-  <si>
-    <t>RES 1K OHM 5% 1/4W AXIAL</t>
-  </si>
-  <si>
-    <t>Stackpole</t>
-  </si>
-  <si>
-    <t>CF14JT10K0</t>
-  </si>
-  <si>
-    <t>CF14JT10K0CT-ND</t>
-  </si>
-  <si>
-    <t>CF14JT1K00</t>
-  </si>
-  <si>
-    <t>CF14JT1K00CT-ND</t>
-  </si>
-  <si>
-    <t>3845-2N3904-ND</t>
-  </si>
-  <si>
-    <t>Fairchild</t>
-  </si>
-  <si>
-    <t>No longer manufactured, but widely available.</t>
-  </si>
-  <si>
-    <t>Multiple subs available</t>
-  </si>
-  <si>
-    <t>Allows for passthrough to use simultaneous with commodore kbd, otherwise can just use standard female or cut leads</t>
-  </si>
-  <si>
-    <t>C64toUSBKeyboard.0.1.gerbers.zip
-or   https://oshpark.com/shared_projects/wqtal8dL</t>
-  </si>
-  <si>
-    <t>v0.1</t>
+    <r>
+      <t xml:space="preserve">24 pin headers to pass control signals from Teensy to PCB.  Not needed with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_PINS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> version of Teensy 4.1</t>
+    </r>
+  </si>
+  <si>
+    <t>20p Female header</t>
+  </si>
+  <si>
+    <t>20 Position Receptacle Connector 0.100" (2.54mm) Through Hole Tin w/ long pins</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -320,6 +385,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -403,9 +474,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -422,6 +490,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -703,22 +774,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" customWidth="1"/>
     <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.44140625" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.5546875" customWidth="1"/>
-    <col min="8" max="8" width="46.5546875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="46.5546875" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="28.8">
@@ -726,7 +797,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -735,16 +806,16 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>58</v>
+      <c r="H1" s="12" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="43.2">
@@ -753,20 +824,20 @@
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="11" t="s">
-        <v>73</v>
+      <c r="H2" s="10" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -779,20 +850,20 @@
       <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>71</v>
+      <c r="G3" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -805,20 +876,20 @@
       <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>62</v>
+      <c r="D4" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>71</v>
+      <c r="G4" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="43.2">
@@ -826,25 +897,25 @@
         <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="G5" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>72</v>
+      <c r="H5" s="10" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.8">
@@ -852,25 +923,25 @@
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>51</v>
+        <v>8</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>50</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>71</v>
+      <c r="H6" s="10" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -878,25 +949,25 @@
         <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>47</v>
+        <v>10</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" s="10" t="s">
         <v>68</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -904,43 +975,43 @@
         <v>1</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>53</v>
+        <v>12</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="11"/>
+      <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="3">
         <v>1</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>17</v>
-      </c>
       <c r="E9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="H9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="28.8">
@@ -948,25 +1019,25 @@
         <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>70</v>
+      <c r="H10" s="10" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -974,73 +1045,128 @@
         <v>1</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>53</v>
+        <v>19</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="11"/>
-    </row>
-    <row r="12" spans="1:8" ht="57.6">
+      <c r="H11" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="43.2">
       <c r="A12" s="3">
         <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="28.8">
+      <c r="A13" s="3">
+        <v>2</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="28.8">
+      <c r="A14" s="3">
+        <v>1</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="5">
+        <v>1</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="5">
-        <v>1</v>
-      </c>
-      <c r="B13" s="4" t="s">
+      <c r="D15" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="7" t="s">
+      <c r="E15" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="G15" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H13" s="11"/>
+      <c r="H15" s="10"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G9" r:id="rId1" xr:uid="{7144FDA5-E356-43DF-BE27-3F95F5BECF2F}"/>
-    <hyperlink ref="G13" r:id="rId2" xr:uid="{95FCFDDA-B004-4794-B971-2F19CB937880}"/>
+    <hyperlink ref="G15" r:id="rId2" xr:uid="{95FCFDDA-B004-4794-B971-2F19CB937880}"/>
     <hyperlink ref="E12" r:id="rId3" display="https://www.pjrc.com/store" xr:uid="{5285EB9C-5A91-4E87-9258-9F3C843B5667}"/>
     <hyperlink ref="F12" r:id="rId4" display="TEENSY41" xr:uid="{6C0173DD-A65A-4B57-839D-2AA7C1441667}"/>
     <hyperlink ref="G12" r:id="rId5" xr:uid="{BBBC10C5-E2D6-4166-95FD-9063E23054B4}"/>
@@ -1049,8 +1175,10 @@
     <hyperlink ref="G4" r:id="rId8" xr:uid="{5E476927-A3C5-4BE9-86C4-68AB3D8EF210}"/>
     <hyperlink ref="G7" r:id="rId9" xr:uid="{A786A0FB-F823-41E2-8E1A-265CB30C9DA0}"/>
     <hyperlink ref="G5" r:id="rId10" xr:uid="{5400FDD2-4DEE-4025-9894-E1E8AF347F0D}"/>
+    <hyperlink ref="G13" r:id="rId11" xr:uid="{7728742E-E7F7-4D85-8B63-CA0216866B7C}"/>
+    <hyperlink ref="G14" r:id="rId12" xr:uid="{9013C50C-7A2D-4122-9151-72A5E73C65FB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>